<commit_message>
first take at some of the custom formats
</commit_message>
<xml_diff>
--- a/tests/issues_format_numbers.xlsx
+++ b/tests/issues_format_numbers.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11210"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10114"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/milan/supplyframe/rsbom/calamine/tests/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5301E47-4C4B-9C4E-9B00-07890B04DC62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A29F77C-C5B9-D74C-9A10-2D171EE95E2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5420" yWindow="3460" windowWidth="30360" windowHeight="20580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5780" yWindow="3720" windowWidth="30360" windowHeight="20580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="issue1" sheetId="6" r:id="rId1"/>
@@ -39,13 +39,22 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="4">
+  <numFmts count="6">
+    <numFmt numFmtId="44" formatCode="_-* #,##0.00\ &quot;RSD&quot;_-;\-* #,##0.00\ &quot;RSD&quot;_-;_-* &quot;-&quot;??\ &quot;RSD&quot;_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="0.000"/>
     <numFmt numFmtId="165" formatCode="#,##0.000000"/>
     <numFmt numFmtId="166" formatCode="[$$-2C09]#,##0.00"/>
     <numFmt numFmtId="167" formatCode="[$₭-454]#,##0.00"/>
+    <numFmt numFmtId="168" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -62,7 +71,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -70,18 +79,34 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Currency" xfId="1" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -384,10 +409,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -422,6 +447,11 @@
         <v>234.23</v>
       </c>
     </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" s="5">
+        <v>7.0000000000000001E-3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
custom formats, storage for builtin formats
</commit_message>
<xml_diff>
--- a/tests/issues_format_numbers.xlsx
+++ b/tests/issues_format_numbers.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/milan/supplyframe/rsbom/calamine/tests/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A29F77C-C5B9-D74C-9A10-2D171EE95E2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7008853-49BE-5849-9E5B-C77D80A8E39B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5780" yWindow="3720" windowWidth="30360" windowHeight="20580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,13 +39,15 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="6">
+  <numFmts count="8">
+    <numFmt numFmtId="6" formatCode="#,##0\ &quot;RSD&quot;;[Red]\-#,##0\ &quot;RSD&quot;"/>
     <numFmt numFmtId="44" formatCode="_-* #,##0.00\ &quot;RSD&quot;_-;\-* #,##0.00\ &quot;RSD&quot;_-;_-* &quot;-&quot;??\ &quot;RSD&quot;_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="0.000"/>
     <numFmt numFmtId="165" formatCode="#,##0.000000"/>
     <numFmt numFmtId="166" formatCode="[$$-2C09]#,##0.00"/>
     <numFmt numFmtId="167" formatCode="[$₭-454]#,##0.00"/>
     <numFmt numFmtId="168" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="170" formatCode="#,##0.0000\ &quot;RSD&quot;"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -95,7 +97,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -104,6 +106,8 @@
     <xf numFmtId="168" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -409,10 +413,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -452,6 +456,26 @@
         <v>7.0000000000000001E-3</v>
       </c>
     </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" s="6">
+        <v>123.4234</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" s="6">
+        <v>-234.56</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" s="7">
+        <v>1234</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" s="3">
+        <v>5445</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
work on formats: percentage
</commit_message>
<xml_diff>
--- a/tests/issues_format_numbers.xlsx
+++ b/tests/issues_format_numbers.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/milan/supplyframe/rsbom/calamine/tests/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D63DF5F-5613-9A43-A780-2CBEAD59D898}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F07096E3-4B4D-9D40-BDE8-C6BBDCD03E3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5480" yWindow="3540" windowWidth="30360" windowHeight="20580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,6 +35,10 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -104,7 +108,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -124,6 +128,7 @@
     <xf numFmtId="189" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="203" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -432,7 +437,7 @@
   <dimension ref="A1:B21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -533,7 +538,9 @@
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A19" s="2"/>
+      <c r="A19" s="17">
+        <v>12.34</v>
+      </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A20" s="16"/>

</xml_diff>